<commit_message>
new version of database and sdf
</commit_message>
<xml_diff>
--- a/notebooks/sdf.xlsx
+++ b/notebooks/sdf.xlsx
@@ -151,6 +151,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -210,8 +211,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -341,382 +346,382 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="0" t="s">
+      <c r="K2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="P2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="Q2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="R2" s="1" t="n">
         <v>1.2</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="S2" s="1" t="n">
         <v>1.2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="0" t="s">
+      <c r="K3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>237</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="P3" s="1" t="n">
         <v>237</v>
       </c>
-      <c r="Q3" s="0" t="n">
+      <c r="Q3" s="1" t="n">
         <v>237</v>
       </c>
-      <c r="R3" s="0" t="n">
+      <c r="R3" s="1" t="n">
         <v>237</v>
       </c>
-      <c r="S3" s="0" t="n">
+      <c r="S3" s="1" t="n">
         <v>237</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="0" t="s">
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="0" t="s">
+      <c r="K4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="M4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="O4" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="P4" s="0" t="n">
+      <c r="P4" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="Q4" s="0" t="n">
+      <c r="Q4" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="R4" s="0" t="n">
+      <c r="R4" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="S4" s="0" t="n">
+      <c r="S4" s="1" t="n">
         <v>0.005</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="0" t="s">
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="0" t="s">
+      <c r="K5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="M5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="O5" s="0" t="n">
+      <c r="O5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="P5" s="0" t="n">
+      <c r="P5" s="1" t="n">
         <v>1.9</v>
       </c>
-      <c r="Q5" s="0" t="n">
+      <c r="Q5" s="1" t="n">
         <v>1.9</v>
       </c>
-      <c r="R5" s="0" t="n">
+      <c r="R5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S5" s="0" t="n">
+      <c r="S5" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="0" t="s">
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="0" t="s">
+      <c r="K6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="M6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="N6" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="O6" s="0" t="n">
+      <c r="O6" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="P6" s="0" t="n">
+      <c r="P6" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="Q6" s="0" t="n">
+      <c r="Q6" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="R6" s="0" t="n">
+      <c r="R6" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="S6" s="0" t="n">
+      <c r="S6" s="1" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="0" t="s">
+      <c r="G7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="N7" s="1" t="n">
         <v>26.6</v>
       </c>
-      <c r="O7" s="0" t="n">
+      <c r="O7" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="P7" s="0" t="n">
+      <c r="P7" s="1" t="n">
         <v>26.6</v>
       </c>
-      <c r="Q7" s="0" t="n">
+      <c r="Q7" s="1" t="n">
         <v>26.6</v>
       </c>
-      <c r="R7" s="0" t="n">
+      <c r="R7" s="1" t="n">
         <v>26.6</v>
       </c>
-      <c r="S7" s="0" t="n">
+      <c r="S7" s="1" t="n">
         <v>26.6</v>
       </c>
     </row>

</xml_diff>